<commit_message>
Added merged + updated datasets
Updated temperature with NOAA data
Added back NAICS 311230
Added merged datasets
</commit_message>
<xml_diff>
--- a/final_data_pipeline/output/311221longform.xlsx
+++ b/final_data_pipeline/output/311221longform.xlsx
@@ -1110,7 +1110,7 @@
         <v>178</v>
       </c>
       <c r="AA2">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB2">
         <v>8000</v>
@@ -1199,7 +1199,7 @@
         <v>178</v>
       </c>
       <c r="AA3">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB3">
         <v>8000</v>
@@ -1291,7 +1291,7 @@
         <v>178</v>
       </c>
       <c r="AA4">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB4">
         <v>8000</v>
@@ -1383,7 +1383,7 @@
         <v>178</v>
       </c>
       <c r="AA5">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB5">
         <v>8000</v>
@@ -1475,7 +1475,7 @@
         <v>178</v>
       </c>
       <c r="AA6">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB6">
         <v>8000</v>
@@ -1567,7 +1567,7 @@
         <v>178</v>
       </c>
       <c r="AA7">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB7">
         <v>8000</v>
@@ -1659,7 +1659,7 @@
         <v>178</v>
       </c>
       <c r="AA8">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB8">
         <v>8000</v>
@@ -1751,7 +1751,7 @@
         <v>178</v>
       </c>
       <c r="AA9">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB9">
         <v>8000</v>
@@ -1849,7 +1849,7 @@
         <v>178</v>
       </c>
       <c r="AA10">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB10">
         <v>8000</v>
@@ -1938,7 +1938,7 @@
         <v>178</v>
       </c>
       <c r="AA11">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB11">
         <v>8000</v>
@@ -2030,7 +2030,7 @@
         <v>178</v>
       </c>
       <c r="AA12">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB12">
         <v>8000</v>
@@ -2128,7 +2128,7 @@
         <v>178</v>
       </c>
       <c r="AA13">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB13">
         <v>8000</v>
@@ -2223,7 +2223,7 @@
         <v>178</v>
       </c>
       <c r="AA14">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB14">
         <v>8000</v>
@@ -2312,7 +2312,7 @@
         <v>178</v>
       </c>
       <c r="AA15">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB15">
         <v>8000</v>
@@ -2401,7 +2401,7 @@
         <v>178</v>
       </c>
       <c r="AA16">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB16">
         <v>8000</v>
@@ -2490,7 +2490,7 @@
         <v>178</v>
       </c>
       <c r="AA17">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB17">
         <v>8000</v>
@@ -2579,7 +2579,7 @@
         <v>178</v>
       </c>
       <c r="AA18">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB18">
         <v>8000</v>
@@ -2671,7 +2671,7 @@
         <v>178</v>
       </c>
       <c r="AA19">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB19">
         <v>8000</v>
@@ -2763,7 +2763,7 @@
         <v>178</v>
       </c>
       <c r="AA20">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB20">
         <v>8000</v>
@@ -2855,7 +2855,7 @@
         <v>178</v>
       </c>
       <c r="AA21">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB21">
         <v>8000</v>
@@ -2947,7 +2947,7 @@
         <v>178</v>
       </c>
       <c r="AA22">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB22">
         <v>8000</v>
@@ -3042,7 +3042,7 @@
         <v>178</v>
       </c>
       <c r="AA23">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB23">
         <v>8000</v>
@@ -3134,7 +3134,7 @@
         <v>178</v>
       </c>
       <c r="AA24">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB24">
         <v>8000</v>
@@ -3232,7 +3232,7 @@
         <v>178</v>
       </c>
       <c r="AA25">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB25">
         <v>8000</v>
@@ -3321,7 +3321,7 @@
         <v>178</v>
       </c>
       <c r="AA26">
-        <v>10</v>
+        <v>1.791666666666668</v>
       </c>
       <c r="AB26">
         <v>8000</v>
@@ -4324,7 +4324,7 @@
         <v>178</v>
       </c>
       <c r="AA37">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB37">
         <v>8000</v>
@@ -4413,7 +4413,7 @@
         <v>178</v>
       </c>
       <c r="AA38">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB38">
         <v>8000</v>
@@ -4502,7 +4502,7 @@
         <v>178</v>
       </c>
       <c r="AA39">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB39">
         <v>8000</v>
@@ -4594,7 +4594,7 @@
         <v>178</v>
       </c>
       <c r="AA40">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB40">
         <v>8000</v>
@@ -4686,7 +4686,7 @@
         <v>178</v>
       </c>
       <c r="AA41">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB41">
         <v>8000</v>
@@ -4778,7 +4778,7 @@
         <v>178</v>
       </c>
       <c r="AA42">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB42">
         <v>8000</v>
@@ -4870,7 +4870,7 @@
         <v>178</v>
       </c>
       <c r="AA43">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB43">
         <v>8000</v>
@@ -4962,7 +4962,7 @@
         <v>178</v>
       </c>
       <c r="AA44">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB44">
         <v>8000</v>
@@ -5054,7 +5054,7 @@
         <v>178</v>
       </c>
       <c r="AA45">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB45">
         <v>8000</v>
@@ -5146,7 +5146,7 @@
         <v>178</v>
       </c>
       <c r="AA46">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB46">
         <v>8000</v>
@@ -5238,7 +5238,7 @@
         <v>178</v>
       </c>
       <c r="AA47">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB47">
         <v>8000</v>
@@ -5327,7 +5327,7 @@
         <v>178</v>
       </c>
       <c r="AA48">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB48">
         <v>8000</v>
@@ -5416,7 +5416,7 @@
         <v>178</v>
       </c>
       <c r="AA49">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB49">
         <v>8000</v>
@@ -5505,7 +5505,7 @@
         <v>178</v>
       </c>
       <c r="AA50">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB50">
         <v>8000</v>
@@ -5594,7 +5594,7 @@
         <v>178</v>
       </c>
       <c r="AA51">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB51">
         <v>8000</v>
@@ -5683,7 +5683,7 @@
         <v>178</v>
       </c>
       <c r="AA52">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB52">
         <v>8000</v>
@@ -5772,7 +5772,7 @@
         <v>178</v>
       </c>
       <c r="AA53">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB53">
         <v>8000</v>
@@ -5864,7 +5864,7 @@
         <v>178</v>
       </c>
       <c r="AA54">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB54">
         <v>8000</v>
@@ -5956,7 +5956,7 @@
         <v>178</v>
       </c>
       <c r="AA55">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB55">
         <v>8000</v>
@@ -6048,7 +6048,7 @@
         <v>178</v>
       </c>
       <c r="AA56">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB56">
         <v>8000</v>
@@ -6146,7 +6146,7 @@
         <v>178</v>
       </c>
       <c r="AA57">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB57">
         <v>8000</v>
@@ -6244,7 +6244,7 @@
         <v>178</v>
       </c>
       <c r="AA58">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB58">
         <v>8000</v>
@@ -6339,7 +6339,7 @@
         <v>178</v>
       </c>
       <c r="AA59">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB59">
         <v>8000</v>
@@ -6431,7 +6431,7 @@
         <v>178</v>
       </c>
       <c r="AA60">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB60">
         <v>8000</v>
@@ -6523,7 +6523,7 @@
         <v>178</v>
       </c>
       <c r="AA61">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB61">
         <v>8000</v>
@@ -6618,7 +6618,7 @@
         <v>178</v>
       </c>
       <c r="AA62">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB62">
         <v>8000</v>
@@ -6710,7 +6710,7 @@
         <v>178</v>
       </c>
       <c r="AA63">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB63">
         <v>8000</v>
@@ -6802,7 +6802,7 @@
         <v>178</v>
       </c>
       <c r="AA64">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB64">
         <v>8000</v>
@@ -6891,7 +6891,7 @@
         <v>178</v>
       </c>
       <c r="AA65">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB65">
         <v>8000</v>
@@ -6980,7 +6980,7 @@
         <v>178</v>
       </c>
       <c r="AA66">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB66">
         <v>8000</v>
@@ -7069,7 +7069,7 @@
         <v>178</v>
       </c>
       <c r="AA67">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB67">
         <v>8000</v>
@@ -7158,7 +7158,7 @@
         <v>178</v>
       </c>
       <c r="AA68">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB68">
         <v>8000</v>
@@ -7250,7 +7250,7 @@
         <v>178</v>
       </c>
       <c r="AA69">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB69">
         <v>8000</v>
@@ -7342,7 +7342,7 @@
         <v>178</v>
       </c>
       <c r="AA70">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB70">
         <v>8000</v>
@@ -7434,7 +7434,7 @@
         <v>178</v>
       </c>
       <c r="AA71">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB71">
         <v>8000</v>
@@ -7523,7 +7523,7 @@
         <v>178</v>
       </c>
       <c r="AA72">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB72">
         <v>8000</v>
@@ -7615,7 +7615,7 @@
         <v>178</v>
       </c>
       <c r="AA73">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB73">
         <v>8000</v>
@@ -7713,7 +7713,7 @@
         <v>178</v>
       </c>
       <c r="AA74">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB74">
         <v>8000</v>
@@ -7805,7 +7805,7 @@
         <v>178</v>
       </c>
       <c r="AA75">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB75">
         <v>8000</v>
@@ -7903,7 +7903,7 @@
         <v>178</v>
       </c>
       <c r="AA76">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB76">
         <v>8000</v>
@@ -7995,7 +7995,7 @@
         <v>178</v>
       </c>
       <c r="AA77">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB77">
         <v>8000</v>
@@ -8087,7 +8087,7 @@
         <v>178</v>
       </c>
       <c r="AA78">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB78">
         <v>8000</v>
@@ -8185,7 +8185,7 @@
         <v>178</v>
       </c>
       <c r="AA79">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB79">
         <v>8000</v>
@@ -8274,7 +8274,7 @@
         <v>178</v>
       </c>
       <c r="AA80">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB80">
         <v>8000</v>
@@ -8363,7 +8363,7 @@
         <v>178</v>
       </c>
       <c r="AA81">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB81">
         <v>8000</v>
@@ -8455,7 +8455,7 @@
         <v>178</v>
       </c>
       <c r="AA82">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB82">
         <v>8000</v>
@@ -8547,7 +8547,7 @@
         <v>178</v>
       </c>
       <c r="AA83">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB83">
         <v>8000</v>
@@ -8639,7 +8639,7 @@
         <v>178</v>
       </c>
       <c r="AA84">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB84">
         <v>8000</v>
@@ -8731,7 +8731,7 @@
         <v>178</v>
       </c>
       <c r="AA85">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB85">
         <v>8000</v>
@@ -8823,7 +8823,7 @@
         <v>178</v>
       </c>
       <c r="AA86">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB86">
         <v>8000</v>
@@ -8921,7 +8921,7 @@
         <v>178</v>
       </c>
       <c r="AA87">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB87">
         <v>8000</v>
@@ -9016,7 +9016,7 @@
         <v>178</v>
       </c>
       <c r="AA88">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB88">
         <v>8000</v>
@@ -9105,7 +9105,7 @@
         <v>178</v>
       </c>
       <c r="AA89">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB89">
         <v>8000</v>
@@ -9194,7 +9194,7 @@
         <v>178</v>
       </c>
       <c r="AA90">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB90">
         <v>8000</v>
@@ -9283,7 +9283,7 @@
         <v>178</v>
       </c>
       <c r="AA91">
-        <v>10</v>
+        <v>19.79629629629628</v>
       </c>
       <c r="AB91">
         <v>8000</v>
@@ -9375,7 +9375,7 @@
         <v>178</v>
       </c>
       <c r="AA92">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB92">
         <v>8000</v>
@@ -9467,7 +9467,7 @@
         <v>178</v>
       </c>
       <c r="AA93">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB93">
         <v>8000</v>
@@ -9559,7 +9559,7 @@
         <v>178</v>
       </c>
       <c r="AA94">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB94">
         <v>8000</v>
@@ -9651,7 +9651,7 @@
         <v>178</v>
       </c>
       <c r="AA95">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB95">
         <v>8000</v>
@@ -9743,7 +9743,7 @@
         <v>178</v>
       </c>
       <c r="AA96">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB96">
         <v>8000</v>
@@ -9835,7 +9835,7 @@
         <v>178</v>
       </c>
       <c r="AA97">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB97">
         <v>8000</v>
@@ -9927,7 +9927,7 @@
         <v>178</v>
       </c>
       <c r="AA98">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB98">
         <v>8000</v>
@@ -10019,7 +10019,7 @@
         <v>178</v>
       </c>
       <c r="AA99">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB99">
         <v>8000</v>
@@ -10111,7 +10111,7 @@
         <v>178</v>
       </c>
       <c r="AA100">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB100">
         <v>8000</v>
@@ -10203,7 +10203,7 @@
         <v>178</v>
       </c>
       <c r="AA101">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB101">
         <v>8000</v>
@@ -10292,7 +10292,7 @@
         <v>178</v>
       </c>
       <c r="AA102">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB102">
         <v>8000</v>
@@ -10384,7 +10384,7 @@
         <v>178</v>
       </c>
       <c r="AA103">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB103">
         <v>8000</v>
@@ -10473,7 +10473,7 @@
         <v>178</v>
       </c>
       <c r="AA104">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB104">
         <v>8000</v>
@@ -10562,7 +10562,7 @@
         <v>178</v>
       </c>
       <c r="AA105">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB105">
         <v>8000</v>
@@ -10651,7 +10651,7 @@
         <v>178</v>
       </c>
       <c r="AA106">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB106">
         <v>8000</v>
@@ -10743,7 +10743,7 @@
         <v>178</v>
       </c>
       <c r="AA107">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB107">
         <v>8000</v>
@@ -10832,7 +10832,7 @@
         <v>178</v>
       </c>
       <c r="AA108">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB108">
         <v>8000</v>
@@ -10921,7 +10921,7 @@
         <v>178</v>
       </c>
       <c r="AA109">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB109">
         <v>8000</v>
@@ -11013,7 +11013,7 @@
         <v>178</v>
       </c>
       <c r="AA110">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB110">
         <v>8000</v>
@@ -11102,7 +11102,7 @@
         <v>178</v>
       </c>
       <c r="AA111">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB111">
         <v>8000</v>
@@ -11194,7 +11194,7 @@
         <v>178</v>
       </c>
       <c r="AA112">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB112">
         <v>8000</v>
@@ -11283,7 +11283,7 @@
         <v>178</v>
       </c>
       <c r="AA113">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB113">
         <v>8000</v>
@@ -11372,7 +11372,7 @@
         <v>178</v>
       </c>
       <c r="AA114">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB114">
         <v>8000</v>
@@ -11461,7 +11461,7 @@
         <v>178</v>
       </c>
       <c r="AA115">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB115">
         <v>8000</v>
@@ -11550,7 +11550,7 @@
         <v>178</v>
       </c>
       <c r="AA116">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB116">
         <v>8000</v>
@@ -11639,7 +11639,7 @@
         <v>178</v>
       </c>
       <c r="AA117">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB117">
         <v>8000</v>
@@ -11728,7 +11728,7 @@
         <v>178</v>
       </c>
       <c r="AA118">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB118">
         <v>8000</v>
@@ -11817,7 +11817,7 @@
         <v>178</v>
       </c>
       <c r="AA119">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB119">
         <v>8000</v>
@@ -11909,7 +11909,7 @@
         <v>178</v>
       </c>
       <c r="AA120">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB120">
         <v>8000</v>
@@ -12001,7 +12001,7 @@
         <v>178</v>
       </c>
       <c r="AA121">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB121">
         <v>8000</v>
@@ -12093,7 +12093,7 @@
         <v>178</v>
       </c>
       <c r="AA122">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB122">
         <v>8000</v>
@@ -12191,7 +12191,7 @@
         <v>178</v>
       </c>
       <c r="AA123">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB123">
         <v>8000</v>
@@ -12289,7 +12289,7 @@
         <v>178</v>
       </c>
       <c r="AA124">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB124">
         <v>8000</v>
@@ -12387,7 +12387,7 @@
         <v>178</v>
       </c>
       <c r="AA125">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB125">
         <v>8000</v>
@@ -12488,7 +12488,7 @@
         <v>178</v>
       </c>
       <c r="AA126">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB126">
         <v>8000</v>
@@ -12583,7 +12583,7 @@
         <v>178</v>
       </c>
       <c r="AA127">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB127">
         <v>8000</v>
@@ -12678,7 +12678,7 @@
         <v>178</v>
       </c>
       <c r="AA128">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB128">
         <v>8000</v>
@@ -12773,7 +12773,7 @@
         <v>178</v>
       </c>
       <c r="AA129">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB129">
         <v>8000</v>
@@ -12865,7 +12865,7 @@
         <v>178</v>
       </c>
       <c r="AA130">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB130">
         <v>8000</v>
@@ -13414,7 +13414,7 @@
         <v>178</v>
       </c>
       <c r="AA136">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB136">
         <v>8000</v>
@@ -13506,7 +13506,7 @@
         <v>178</v>
       </c>
       <c r="AA137">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB137">
         <v>8000</v>
@@ -13604,7 +13604,7 @@
         <v>178</v>
       </c>
       <c r="AA138">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB138">
         <v>8000</v>
@@ -13696,7 +13696,7 @@
         <v>178</v>
       </c>
       <c r="AA139">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB139">
         <v>8000</v>
@@ -13788,7 +13788,7 @@
         <v>178</v>
       </c>
       <c r="AA140">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB140">
         <v>8000</v>
@@ -13880,7 +13880,7 @@
         <v>178</v>
       </c>
       <c r="AA141">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB141">
         <v>8000</v>
@@ -13972,7 +13972,7 @@
         <v>178</v>
       </c>
       <c r="AA142">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB142">
         <v>8000</v>
@@ -14064,7 +14064,7 @@
         <v>178</v>
       </c>
       <c r="AA143">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB143">
         <v>8000</v>
@@ -14156,7 +14156,7 @@
         <v>178</v>
       </c>
       <c r="AA144">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB144">
         <v>8000</v>
@@ -14248,7 +14248,7 @@
         <v>178</v>
       </c>
       <c r="AA145">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB145">
         <v>8000</v>
@@ -14346,7 +14346,7 @@
         <v>178</v>
       </c>
       <c r="AA146">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB146">
         <v>8000</v>
@@ -14444,7 +14444,7 @@
         <v>178</v>
       </c>
       <c r="AA147">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB147">
         <v>8000</v>
@@ -14542,7 +14542,7 @@
         <v>178</v>
       </c>
       <c r="AA148">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB148">
         <v>8000</v>
@@ -14640,7 +14640,7 @@
         <v>178</v>
       </c>
       <c r="AA149">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB149">
         <v>8000</v>
@@ -14738,7 +14738,7 @@
         <v>178</v>
       </c>
       <c r="AA150">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB150">
         <v>8000</v>
@@ -14836,7 +14836,7 @@
         <v>178</v>
       </c>
       <c r="AA151">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB151">
         <v>8000</v>
@@ -14928,7 +14928,7 @@
         <v>178</v>
       </c>
       <c r="AA152">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB152">
         <v>8000</v>
@@ -15017,7 +15017,7 @@
         <v>178</v>
       </c>
       <c r="AA153">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB153">
         <v>8000</v>
@@ -15109,7 +15109,7 @@
         <v>178</v>
       </c>
       <c r="AA154">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB154">
         <v>8000</v>
@@ -15198,7 +15198,7 @@
         <v>178</v>
       </c>
       <c r="AA155">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB155">
         <v>8000</v>
@@ -15287,7 +15287,7 @@
         <v>178</v>
       </c>
       <c r="AA156">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB156">
         <v>8000</v>
@@ -15379,7 +15379,7 @@
         <v>178</v>
       </c>
       <c r="AA157">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB157">
         <v>8000</v>
@@ -15471,7 +15471,7 @@
         <v>178</v>
       </c>
       <c r="AA158">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB158">
         <v>8000</v>
@@ -15563,7 +15563,7 @@
         <v>178</v>
       </c>
       <c r="AA159">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB159">
         <v>8000</v>
@@ -15655,7 +15655,7 @@
         <v>178</v>
       </c>
       <c r="AA160">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB160">
         <v>8000</v>
@@ -15744,7 +15744,7 @@
         <v>178</v>
       </c>
       <c r="AA161">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB161">
         <v>8000</v>
@@ -15833,7 +15833,7 @@
         <v>178</v>
       </c>
       <c r="AA162">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB162">
         <v>8000</v>
@@ -15922,7 +15922,7 @@
         <v>178</v>
       </c>
       <c r="AA163">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB163">
         <v>8000</v>
@@ -16011,7 +16011,7 @@
         <v>178</v>
       </c>
       <c r="AA164">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB164">
         <v>8000</v>
@@ -16100,7 +16100,7 @@
         <v>178</v>
       </c>
       <c r="AA165">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB165">
         <v>8000</v>
@@ -16189,7 +16189,7 @@
         <v>178</v>
       </c>
       <c r="AA166">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB166">
         <v>8000</v>
@@ -16278,7 +16278,7 @@
         <v>178</v>
       </c>
       <c r="AA167">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB167">
         <v>8000</v>
@@ -16367,7 +16367,7 @@
         <v>178</v>
       </c>
       <c r="AA168">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB168">
         <v>8000</v>
@@ -16456,7 +16456,7 @@
         <v>178</v>
       </c>
       <c r="AA169">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB169">
         <v>8000</v>
@@ -16545,7 +16545,7 @@
         <v>178</v>
       </c>
       <c r="AA170">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB170">
         <v>8000</v>
@@ -16634,7 +16634,7 @@
         <v>178</v>
       </c>
       <c r="AA171">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB171">
         <v>8000</v>
@@ -16723,7 +16723,7 @@
         <v>178</v>
       </c>
       <c r="AA172">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB172">
         <v>8000</v>
@@ -16815,7 +16815,7 @@
         <v>178</v>
       </c>
       <c r="AA173">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB173">
         <v>8000</v>
@@ -16913,7 +16913,7 @@
         <v>178</v>
       </c>
       <c r="AA174">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB174">
         <v>8000</v>
@@ -17005,7 +17005,7 @@
         <v>178</v>
       </c>
       <c r="AA175">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB175">
         <v>8000</v>
@@ -17097,7 +17097,7 @@
         <v>178</v>
       </c>
       <c r="AA176">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB176">
         <v>8000</v>
@@ -17189,7 +17189,7 @@
         <v>178</v>
       </c>
       <c r="AA177">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB177">
         <v>8000</v>
@@ -17278,7 +17278,7 @@
         <v>178</v>
       </c>
       <c r="AA178">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB178">
         <v>8000</v>
@@ -17367,7 +17367,7 @@
         <v>178</v>
       </c>
       <c r="AA179">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB179">
         <v>8000</v>
@@ -17459,7 +17459,7 @@
         <v>178</v>
       </c>
       <c r="AA180">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB180">
         <v>8000</v>
@@ -18922,7 +18922,7 @@
         <v>178</v>
       </c>
       <c r="AA196">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB196">
         <v>8000</v>
@@ -19011,7 +19011,7 @@
         <v>178</v>
       </c>
       <c r="AA197">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB197">
         <v>8000</v>
@@ -19100,7 +19100,7 @@
         <v>178</v>
       </c>
       <c r="AA198">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB198">
         <v>8000</v>
@@ -19189,7 +19189,7 @@
         <v>178</v>
       </c>
       <c r="AA199">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB199">
         <v>8000</v>
@@ -19281,7 +19281,7 @@
         <v>178</v>
       </c>
       <c r="AA200">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB200">
         <v>8000</v>
@@ -19379,7 +19379,7 @@
         <v>178</v>
       </c>
       <c r="AA201">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB201">
         <v>8000</v>
@@ -19471,7 +19471,7 @@
         <v>178</v>
       </c>
       <c r="AA202">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB202">
         <v>8000</v>
@@ -19563,7 +19563,7 @@
         <v>178</v>
       </c>
       <c r="AA203">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB203">
         <v>8000</v>
@@ -19655,7 +19655,7 @@
         <v>178</v>
       </c>
       <c r="AA204">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB204">
         <v>8000</v>
@@ -19747,7 +19747,7 @@
         <v>178</v>
       </c>
       <c r="AA205">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB205">
         <v>8000</v>
@@ -19836,7 +19836,7 @@
         <v>178</v>
       </c>
       <c r="AA206">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB206">
         <v>8000</v>
@@ -19925,7 +19925,7 @@
         <v>178</v>
       </c>
       <c r="AA207">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB207">
         <v>8000</v>
@@ -20014,7 +20014,7 @@
         <v>178</v>
       </c>
       <c r="AA208">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB208">
         <v>8000</v>
@@ -20103,7 +20103,7 @@
         <v>178</v>
       </c>
       <c r="AA209">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB209">
         <v>8000</v>
@@ -20195,7 +20195,7 @@
         <v>178</v>
       </c>
       <c r="AA210">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB210">
         <v>8000</v>
@@ -20287,7 +20287,7 @@
         <v>178</v>
       </c>
       <c r="AA211">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB211">
         <v>8000</v>
@@ -20385,7 +20385,7 @@
         <v>178</v>
       </c>
       <c r="AA212">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB212">
         <v>8000</v>
@@ -20483,7 +20483,7 @@
         <v>178</v>
       </c>
       <c r="AA213">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB213">
         <v>8000</v>
@@ -20581,7 +20581,7 @@
         <v>178</v>
       </c>
       <c r="AA214">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB214">
         <v>8000</v>
@@ -20673,7 +20673,7 @@
         <v>178</v>
       </c>
       <c r="AA215">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB215">
         <v>8000</v>
@@ -20762,7 +20762,7 @@
         <v>178</v>
       </c>
       <c r="AA216">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB216">
         <v>8000</v>
@@ -20851,7 +20851,7 @@
         <v>178</v>
       </c>
       <c r="AA217">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB217">
         <v>8000</v>
@@ -20940,7 +20940,7 @@
         <v>178</v>
       </c>
       <c r="AA218">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB218">
         <v>8000</v>
@@ -21029,7 +21029,7 @@
         <v>178</v>
       </c>
       <c r="AA219">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB219">
         <v>8000</v>
@@ -21118,7 +21118,7 @@
         <v>178</v>
       </c>
       <c r="AA220">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB220">
         <v>8000</v>
@@ -21207,7 +21207,7 @@
         <v>178</v>
       </c>
       <c r="AA221">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB221">
         <v>8000</v>
@@ -21296,7 +21296,7 @@
         <v>178</v>
       </c>
       <c r="AA222">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB222">
         <v>8000</v>
@@ -21385,7 +21385,7 @@
         <v>178</v>
       </c>
       <c r="AA223">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB223">
         <v>8000</v>
@@ -21477,7 +21477,7 @@
         <v>178</v>
       </c>
       <c r="AA224">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB224">
         <v>8000</v>
@@ -21569,7 +21569,7 @@
         <v>178</v>
       </c>
       <c r="AA225">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB225">
         <v>8000</v>
@@ -21661,7 +21661,7 @@
         <v>178</v>
       </c>
       <c r="AA226">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB226">
         <v>8000</v>
@@ -21753,7 +21753,7 @@
         <v>178</v>
       </c>
       <c r="AA227">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB227">
         <v>8000</v>
@@ -21845,7 +21845,7 @@
         <v>178</v>
       </c>
       <c r="AA228">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB228">
         <v>8000</v>
@@ -21934,7 +21934,7 @@
         <v>178</v>
       </c>
       <c r="AA229">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB229">
         <v>8000</v>
@@ -22023,7 +22023,7 @@
         <v>178</v>
       </c>
       <c r="AA230">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB230">
         <v>8000</v>
@@ -22112,7 +22112,7 @@
         <v>178</v>
       </c>
       <c r="AA231">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB231">
         <v>8000</v>
@@ -22204,7 +22204,7 @@
         <v>178</v>
       </c>
       <c r="AA232">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB232">
         <v>8000</v>
@@ -22293,7 +22293,7 @@
         <v>178</v>
       </c>
       <c r="AA233">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB233">
         <v>8000</v>
@@ -22385,7 +22385,7 @@
         <v>178</v>
       </c>
       <c r="AA234">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB234">
         <v>8000</v>
@@ -22483,7 +22483,7 @@
         <v>178</v>
       </c>
       <c r="AA235">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB235">
         <v>8000</v>
@@ -22581,7 +22581,7 @@
         <v>178</v>
       </c>
       <c r="AA236">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB236">
         <v>8000</v>
@@ -22679,7 +22679,7 @@
         <v>178</v>
       </c>
       <c r="AA237">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB237">
         <v>8000</v>
@@ -22771,7 +22771,7 @@
         <v>178</v>
       </c>
       <c r="AA238">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB238">
         <v>8000</v>
@@ -22863,7 +22863,7 @@
         <v>178</v>
       </c>
       <c r="AA239">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB239">
         <v>8000</v>
@@ -22955,7 +22955,7 @@
         <v>178</v>
       </c>
       <c r="AA240">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB240">
         <v>8000</v>
@@ -23047,7 +23047,7 @@
         <v>178</v>
       </c>
       <c r="AA241">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB241">
         <v>8000</v>
@@ -23145,7 +23145,7 @@
         <v>178</v>
       </c>
       <c r="AA242">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB242">
         <v>8000</v>
@@ -23237,7 +23237,7 @@
         <v>178</v>
       </c>
       <c r="AA243">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB243">
         <v>8000</v>
@@ -23335,7 +23335,7 @@
         <v>178</v>
       </c>
       <c r="AA244">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB244">
         <v>8000</v>
@@ -23427,7 +23427,7 @@
         <v>178</v>
       </c>
       <c r="AA245">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB245">
         <v>8000</v>
@@ -24439,7 +24439,7 @@
         <v>178</v>
       </c>
       <c r="AA256">
-        <v>10</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="AB256">
         <v>8000</v>
@@ -24537,7 +24537,7 @@
         <v>178</v>
       </c>
       <c r="AA257">
-        <v>10</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="AB257">
         <v>8000</v>
@@ -24626,7 +24626,7 @@
         <v>178</v>
       </c>
       <c r="AA258">
-        <v>10</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="AB258">
         <v>8000</v>
@@ -24715,7 +24715,7 @@
         <v>178</v>
       </c>
       <c r="AA259">
-        <v>10</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="AB259">
         <v>8000</v>
@@ -24807,7 +24807,7 @@
         <v>178</v>
       </c>
       <c r="AA260">
-        <v>10</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="AB260">
         <v>8000</v>
@@ -25819,7 +25819,7 @@
         <v>178</v>
       </c>
       <c r="AA271">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB271">
         <v>8000</v>
@@ -25911,7 +25911,7 @@
         <v>178</v>
       </c>
       <c r="AA272">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB272">
         <v>8000</v>
@@ -26003,7 +26003,7 @@
         <v>178</v>
       </c>
       <c r="AA273">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB273">
         <v>8000</v>
@@ -26092,7 +26092,7 @@
         <v>178</v>
       </c>
       <c r="AA274">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB274">
         <v>8000</v>
@@ -26181,7 +26181,7 @@
         <v>178</v>
       </c>
       <c r="AA275">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB275">
         <v>8000</v>
@@ -26270,7 +26270,7 @@
         <v>178</v>
       </c>
       <c r="AA276">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB276">
         <v>8000</v>
@@ -26359,7 +26359,7 @@
         <v>178</v>
       </c>
       <c r="AA277">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB277">
         <v>8000</v>
@@ -26451,7 +26451,7 @@
         <v>178</v>
       </c>
       <c r="AA278">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB278">
         <v>8000</v>
@@ -26543,7 +26543,7 @@
         <v>178</v>
       </c>
       <c r="AA279">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB279">
         <v>8000</v>
@@ -26632,7 +26632,7 @@
         <v>178</v>
       </c>
       <c r="AA280">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB280">
         <v>8000</v>
@@ -26721,7 +26721,7 @@
         <v>178</v>
       </c>
       <c r="AA281">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB281">
         <v>8000</v>
@@ -26813,7 +26813,7 @@
         <v>178</v>
       </c>
       <c r="AA282">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB282">
         <v>8000</v>
@@ -26902,7 +26902,7 @@
         <v>178</v>
       </c>
       <c r="AA283">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB283">
         <v>8000</v>
@@ -26991,7 +26991,7 @@
         <v>178</v>
       </c>
       <c r="AA284">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB284">
         <v>8000</v>
@@ -27083,7 +27083,7 @@
         <v>178</v>
       </c>
       <c r="AA285">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB285">
         <v>8000</v>
@@ -27175,7 +27175,7 @@
         <v>178</v>
       </c>
       <c r="AA286">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB286">
         <v>8000</v>
@@ -27273,7 +27273,7 @@
         <v>178</v>
       </c>
       <c r="AA287">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB287">
         <v>8000</v>
@@ -27365,7 +27365,7 @@
         <v>178</v>
       </c>
       <c r="AA288">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB288">
         <v>8000</v>
@@ -27457,7 +27457,7 @@
         <v>178</v>
       </c>
       <c r="AA289">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB289">
         <v>8000</v>
@@ -27546,7 +27546,7 @@
         <v>178</v>
       </c>
       <c r="AA290">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB290">
         <v>8000</v>
@@ -27635,7 +27635,7 @@
         <v>178</v>
       </c>
       <c r="AA291">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB291">
         <v>8000</v>
@@ -27727,7 +27727,7 @@
         <v>178</v>
       </c>
       <c r="AA292">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB292">
         <v>8000</v>
@@ -27825,7 +27825,7 @@
         <v>178</v>
       </c>
       <c r="AA293">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB293">
         <v>8000</v>
@@ -27923,7 +27923,7 @@
         <v>178</v>
       </c>
       <c r="AA294">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB294">
         <v>8000</v>
@@ -28021,7 +28021,7 @@
         <v>178</v>
       </c>
       <c r="AA295">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB295">
         <v>8000</v>
@@ -33164,7 +33164,7 @@
         <v>178</v>
       </c>
       <c r="AA351">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB351">
         <v>8000</v>
@@ -33253,7 +33253,7 @@
         <v>178</v>
       </c>
       <c r="AA352">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB352">
         <v>8000</v>
@@ -33342,7 +33342,7 @@
         <v>178</v>
       </c>
       <c r="AA353">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB353">
         <v>8000</v>
@@ -33431,7 +33431,7 @@
         <v>178</v>
       </c>
       <c r="AA354">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB354">
         <v>8000</v>
@@ -33520,7 +33520,7 @@
         <v>178</v>
       </c>
       <c r="AA355">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB355">
         <v>8000</v>
@@ -33609,7 +33609,7 @@
         <v>178</v>
       </c>
       <c r="AA356">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB356">
         <v>8000</v>
@@ -33698,7 +33698,7 @@
         <v>178</v>
       </c>
       <c r="AA357">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB357">
         <v>8000</v>
@@ -33790,7 +33790,7 @@
         <v>178</v>
       </c>
       <c r="AA358">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB358">
         <v>8000</v>
@@ -33888,7 +33888,7 @@
         <v>178</v>
       </c>
       <c r="AA359">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB359">
         <v>8000</v>
@@ -33986,7 +33986,7 @@
         <v>178</v>
       </c>
       <c r="AA360">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB360">
         <v>8000</v>
@@ -34084,7 +34084,7 @@
         <v>178</v>
       </c>
       <c r="AA361">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB361">
         <v>8000</v>
@@ -34182,7 +34182,7 @@
         <v>178</v>
       </c>
       <c r="AA362">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB362">
         <v>8000</v>
@@ -34280,7 +34280,7 @@
         <v>178</v>
       </c>
       <c r="AA363">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB363">
         <v>8000</v>
@@ -34378,7 +34378,7 @@
         <v>178</v>
       </c>
       <c r="AA364">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB364">
         <v>8000</v>
@@ -34476,7 +34476,7 @@
         <v>178</v>
       </c>
       <c r="AA365">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB365">
         <v>8000</v>
@@ -34574,7 +34574,7 @@
         <v>178</v>
       </c>
       <c r="AA366">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB366">
         <v>8000</v>
@@ -34672,7 +34672,7 @@
         <v>178</v>
       </c>
       <c r="AA367">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB367">
         <v>8000</v>
@@ -34761,7 +34761,7 @@
         <v>178</v>
       </c>
       <c r="AA368">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB368">
         <v>8000</v>
@@ -34850,7 +34850,7 @@
         <v>178</v>
       </c>
       <c r="AA369">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB369">
         <v>8000</v>
@@ -34942,7 +34942,7 @@
         <v>178</v>
       </c>
       <c r="AA370">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB370">
         <v>8000</v>
@@ -35034,7 +35034,7 @@
         <v>178</v>
       </c>
       <c r="AA371">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB371">
         <v>8000</v>
@@ -35126,7 +35126,7 @@
         <v>178</v>
       </c>
       <c r="AA372">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB372">
         <v>8000</v>
@@ -35218,7 +35218,7 @@
         <v>178</v>
       </c>
       <c r="AA373">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB373">
         <v>8000</v>
@@ -35310,7 +35310,7 @@
         <v>178</v>
       </c>
       <c r="AA374">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB374">
         <v>8000</v>
@@ -35402,7 +35402,7 @@
         <v>178</v>
       </c>
       <c r="AA375">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB375">
         <v>8000</v>
@@ -35494,7 +35494,7 @@
         <v>178</v>
       </c>
       <c r="AA376">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB376">
         <v>8000</v>
@@ -35586,7 +35586,7 @@
         <v>178</v>
       </c>
       <c r="AA377">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB377">
         <v>8000</v>
@@ -35678,7 +35678,7 @@
         <v>178</v>
       </c>
       <c r="AA378">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB378">
         <v>8000</v>
@@ -35770,7 +35770,7 @@
         <v>178</v>
       </c>
       <c r="AA379">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB379">
         <v>8000</v>
@@ -35862,7 +35862,7 @@
         <v>178</v>
       </c>
       <c r="AA380">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB380">
         <v>8000</v>
@@ -35954,7 +35954,7 @@
         <v>178</v>
       </c>
       <c r="AA381">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB381">
         <v>8000</v>
@@ -36043,7 +36043,7 @@
         <v>178</v>
       </c>
       <c r="AA382">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB382">
         <v>8000</v>
@@ -36132,7 +36132,7 @@
         <v>178</v>
       </c>
       <c r="AA383">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB383">
         <v>8000</v>
@@ -36221,7 +36221,7 @@
         <v>178</v>
       </c>
       <c r="AA384">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB384">
         <v>8000</v>
@@ -36310,7 +36310,7 @@
         <v>178</v>
       </c>
       <c r="AA385">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB385">
         <v>8000</v>
@@ -36399,7 +36399,7 @@
         <v>178</v>
       </c>
       <c r="AA386">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB386">
         <v>8000</v>
@@ -36491,7 +36491,7 @@
         <v>178</v>
       </c>
       <c r="AA387">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB387">
         <v>8000</v>
@@ -36580,7 +36580,7 @@
         <v>178</v>
       </c>
       <c r="AA388">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB388">
         <v>8000</v>
@@ -36672,7 +36672,7 @@
         <v>178</v>
       </c>
       <c r="AA389">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB389">
         <v>8000</v>
@@ -36764,7 +36764,7 @@
         <v>178</v>
       </c>
       <c r="AA390">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB390">
         <v>8000</v>
@@ -36856,7 +36856,7 @@
         <v>178</v>
       </c>
       <c r="AA391">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB391">
         <v>8000</v>
@@ -36948,7 +36948,7 @@
         <v>178</v>
       </c>
       <c r="AA392">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB392">
         <v>8000</v>
@@ -37040,7 +37040,7 @@
         <v>178</v>
       </c>
       <c r="AA393">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB393">
         <v>8000</v>
@@ -37129,7 +37129,7 @@
         <v>178</v>
       </c>
       <c r="AA394">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB394">
         <v>8000</v>
@@ -37221,7 +37221,7 @@
         <v>178</v>
       </c>
       <c r="AA395">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB395">
         <v>8000</v>
@@ -37313,7 +37313,7 @@
         <v>178</v>
       </c>
       <c r="AA396">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB396">
         <v>8000</v>
@@ -37405,7 +37405,7 @@
         <v>178</v>
       </c>
       <c r="AA397">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB397">
         <v>8000</v>
@@ -37494,7 +37494,7 @@
         <v>178</v>
       </c>
       <c r="AA398">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB398">
         <v>8000</v>
@@ -37583,7 +37583,7 @@
         <v>178</v>
       </c>
       <c r="AA399">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB399">
         <v>8000</v>
@@ -37672,7 +37672,7 @@
         <v>178</v>
       </c>
       <c r="AA400">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB400">
         <v>8000</v>
@@ -37764,7 +37764,7 @@
         <v>178</v>
       </c>
       <c r="AA401">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB401">
         <v>8000</v>
@@ -37859,7 +37859,7 @@
         <v>178</v>
       </c>
       <c r="AA402">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB402">
         <v>8000</v>
@@ -37948,7 +37948,7 @@
         <v>178</v>
       </c>
       <c r="AA403">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB403">
         <v>8000</v>
@@ -38040,7 +38040,7 @@
         <v>178</v>
       </c>
       <c r="AA404">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB404">
         <v>8000</v>
@@ -38129,7 +38129,7 @@
         <v>178</v>
       </c>
       <c r="AA405">
-        <v>10</v>
+        <v>12.93898809523811</v>
       </c>
       <c r="AB405">
         <v>8000</v>
@@ -38221,7 +38221,7 @@
         <v>178</v>
       </c>
       <c r="AA406">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB406">
         <v>8000</v>
@@ -38319,7 +38319,7 @@
         <v>178</v>
       </c>
       <c r="AA407">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB407">
         <v>8000</v>
@@ -38417,7 +38417,7 @@
         <v>178</v>
       </c>
       <c r="AA408">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB408">
         <v>8000</v>
@@ -38512,7 +38512,7 @@
         <v>178</v>
       </c>
       <c r="AA409">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB409">
         <v>8000</v>
@@ -38601,7 +38601,7 @@
         <v>178</v>
       </c>
       <c r="AA410">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB410">
         <v>8000</v>
@@ -38690,7 +38690,7 @@
         <v>178</v>
       </c>
       <c r="AA411">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB411">
         <v>8000</v>
@@ -38779,7 +38779,7 @@
         <v>178</v>
       </c>
       <c r="AA412">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB412">
         <v>8000</v>
@@ -38868,7 +38868,7 @@
         <v>178</v>
       </c>
       <c r="AA413">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB413">
         <v>8000</v>
@@ -38960,7 +38960,7 @@
         <v>178</v>
       </c>
       <c r="AA414">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB414">
         <v>8000</v>
@@ -39052,7 +39052,7 @@
         <v>178</v>
       </c>
       <c r="AA415">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB415">
         <v>8000</v>
@@ -39141,7 +39141,7 @@
         <v>178</v>
       </c>
       <c r="AA416">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB416">
         <v>8000</v>
@@ -39233,7 +39233,7 @@
         <v>178</v>
       </c>
       <c r="AA417">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB417">
         <v>8000</v>
@@ -39325,7 +39325,7 @@
         <v>178</v>
       </c>
       <c r="AA418">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB418">
         <v>8000</v>
@@ -39417,7 +39417,7 @@
         <v>178</v>
       </c>
       <c r="AA419">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB419">
         <v>8000</v>
@@ -39509,7 +39509,7 @@
         <v>178</v>
       </c>
       <c r="AA420">
-        <v>10</v>
+        <v>13.76976495726495</v>
       </c>
       <c r="AB420">
         <v>8000</v>
@@ -39598,7 +39598,7 @@
         <v>178</v>
       </c>
       <c r="AA421">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB421">
         <v>8000</v>
@@ -39687,7 +39687,7 @@
         <v>178</v>
       </c>
       <c r="AA422">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB422">
         <v>8000</v>
@@ -39776,7 +39776,7 @@
         <v>178</v>
       </c>
       <c r="AA423">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB423">
         <v>8000</v>
@@ -39865,7 +39865,7 @@
         <v>178</v>
       </c>
       <c r="AA424">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB424">
         <v>8000</v>
@@ -39957,7 +39957,7 @@
         <v>178</v>
       </c>
       <c r="AA425">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB425">
         <v>8000</v>
@@ -40046,7 +40046,7 @@
         <v>178</v>
       </c>
       <c r="AA426">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB426">
         <v>8000</v>
@@ -40135,7 +40135,7 @@
         <v>178</v>
       </c>
       <c r="AA427">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB427">
         <v>8000</v>
@@ -40227,7 +40227,7 @@
         <v>178</v>
       </c>
       <c r="AA428">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB428">
         <v>8000</v>
@@ -40322,7 +40322,7 @@
         <v>178</v>
       </c>
       <c r="AA429">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB429">
         <v>8000</v>
@@ -40411,7 +40411,7 @@
         <v>178</v>
       </c>
       <c r="AA430">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB430">
         <v>8000</v>
@@ -40503,7 +40503,7 @@
         <v>178</v>
       </c>
       <c r="AA431">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB431">
         <v>8000</v>
@@ -40601,7 +40601,7 @@
         <v>178</v>
       </c>
       <c r="AA432">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB432">
         <v>8000</v>
@@ -40699,7 +40699,7 @@
         <v>178</v>
       </c>
       <c r="AA433">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB433">
         <v>8000</v>
@@ -40791,7 +40791,7 @@
         <v>178</v>
       </c>
       <c r="AA434">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB434">
         <v>8000</v>
@@ -40886,7 +40886,7 @@
         <v>178</v>
       </c>
       <c r="AA435">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB435">
         <v>8000</v>
@@ -40978,7 +40978,7 @@
         <v>178</v>
       </c>
       <c r="AA436">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB436">
         <v>8000</v>
@@ -41076,7 +41076,7 @@
         <v>178</v>
       </c>
       <c r="AA437">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB437">
         <v>8000</v>
@@ -41174,7 +41174,7 @@
         <v>178</v>
       </c>
       <c r="AA438">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB438">
         <v>8000</v>
@@ -41266,7 +41266,7 @@
         <v>178</v>
       </c>
       <c r="AA439">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB439">
         <v>8000</v>
@@ -41358,7 +41358,7 @@
         <v>178</v>
       </c>
       <c r="AA440">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB440">
         <v>8000</v>
@@ -41450,7 +41450,7 @@
         <v>178</v>
       </c>
       <c r="AA441">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB441">
         <v>8000</v>
@@ -41542,7 +41542,7 @@
         <v>178</v>
       </c>
       <c r="AA442">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB442">
         <v>8000</v>
@@ -41634,7 +41634,7 @@
         <v>178</v>
       </c>
       <c r="AA443">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB443">
         <v>8000</v>
@@ -41726,7 +41726,7 @@
         <v>178</v>
       </c>
       <c r="AA444">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB444">
         <v>8000</v>
@@ -41818,7 +41818,7 @@
         <v>178</v>
       </c>
       <c r="AA445">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB445">
         <v>8000</v>
@@ -41910,7 +41910,7 @@
         <v>178</v>
       </c>
       <c r="AA446">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB446">
         <v>8000</v>
@@ -42002,7 +42002,7 @@
         <v>178</v>
       </c>
       <c r="AA447">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB447">
         <v>8000</v>
@@ -42094,7 +42094,7 @@
         <v>178</v>
       </c>
       <c r="AA448">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB448">
         <v>8000</v>
@@ -42186,7 +42186,7 @@
         <v>178</v>
       </c>
       <c r="AA449">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB449">
         <v>8000</v>
@@ -42278,7 +42278,7 @@
         <v>178</v>
       </c>
       <c r="AA450">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB450">
         <v>8000</v>
@@ -42370,7 +42370,7 @@
         <v>178</v>
       </c>
       <c r="AA451">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB451">
         <v>8000</v>
@@ -42459,7 +42459,7 @@
         <v>178</v>
       </c>
       <c r="AA452">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB452">
         <v>8000</v>
@@ -42551,7 +42551,7 @@
         <v>178</v>
       </c>
       <c r="AA453">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB453">
         <v>8000</v>
@@ -42643,7 +42643,7 @@
         <v>178</v>
       </c>
       <c r="AA454">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB454">
         <v>8000</v>
@@ -42735,7 +42735,7 @@
         <v>178</v>
       </c>
       <c r="AA455">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB455">
         <v>8000</v>
@@ -42827,7 +42827,7 @@
         <v>178</v>
       </c>
       <c r="AA456">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB456">
         <v>8000</v>
@@ -42919,7 +42919,7 @@
         <v>178</v>
       </c>
       <c r="AA457">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB457">
         <v>8000</v>
@@ -43014,7 +43014,7 @@
         <v>178</v>
       </c>
       <c r="AA458">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB458">
         <v>8000</v>
@@ -43103,7 +43103,7 @@
         <v>178</v>
       </c>
       <c r="AA459">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB459">
         <v>8000</v>
@@ -43192,7 +43192,7 @@
         <v>178</v>
       </c>
       <c r="AA460">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB460">
         <v>8000</v>
@@ -43281,7 +43281,7 @@
         <v>178</v>
       </c>
       <c r="AA461">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB461">
         <v>8000</v>
@@ -43370,7 +43370,7 @@
         <v>178</v>
       </c>
       <c r="AA462">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB462">
         <v>8000</v>
@@ -43459,7 +43459,7 @@
         <v>178</v>
       </c>
       <c r="AA463">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB463">
         <v>8000</v>
@@ -43548,7 +43548,7 @@
         <v>178</v>
       </c>
       <c r="AA464">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB464">
         <v>8000</v>
@@ -43637,7 +43637,7 @@
         <v>178</v>
       </c>
       <c r="AA465">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB465">
         <v>8000</v>
@@ -43729,7 +43729,7 @@
         <v>178</v>
       </c>
       <c r="AA466">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB466">
         <v>8000</v>
@@ -43821,7 +43821,7 @@
         <v>178</v>
       </c>
       <c r="AA467">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB467">
         <v>8000</v>
@@ -43913,7 +43913,7 @@
         <v>178</v>
       </c>
       <c r="AA468">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB468">
         <v>8000</v>
@@ -44005,7 +44005,7 @@
         <v>178</v>
       </c>
       <c r="AA469">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB469">
         <v>8000</v>
@@ -44097,7 +44097,7 @@
         <v>178</v>
       </c>
       <c r="AA470">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB470">
         <v>8000</v>
@@ -44189,7 +44189,7 @@
         <v>178</v>
       </c>
       <c r="AA471">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB471">
         <v>8000</v>
@@ -44281,7 +44281,7 @@
         <v>178</v>
       </c>
       <c r="AA472">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB472">
         <v>8000</v>
@@ -44376,7 +44376,7 @@
         <v>178</v>
       </c>
       <c r="AA473">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB473">
         <v>8000</v>
@@ -44465,7 +44465,7 @@
         <v>178</v>
       </c>
       <c r="AA474">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB474">
         <v>8000</v>
@@ -44554,7 +44554,7 @@
         <v>178</v>
       </c>
       <c r="AA475">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB475">
         <v>8000</v>
@@ -44643,7 +44643,7 @@
         <v>178</v>
       </c>
       <c r="AA476">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB476">
         <v>8000</v>
@@ -44735,7 +44735,7 @@
         <v>178</v>
       </c>
       <c r="AA477">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB477">
         <v>8000</v>
@@ -44827,7 +44827,7 @@
         <v>178</v>
       </c>
       <c r="AA478">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB478">
         <v>8000</v>
@@ -44925,7 +44925,7 @@
         <v>178</v>
       </c>
       <c r="AA479">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB479">
         <v>8000</v>
@@ -45023,7 +45023,7 @@
         <v>178</v>
       </c>
       <c r="AA480">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB480">
         <v>8000</v>
@@ -45115,7 +45115,7 @@
         <v>178</v>
       </c>
       <c r="AA481">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB481">
         <v>8000</v>
@@ -45213,7 +45213,7 @@
         <v>178</v>
       </c>
       <c r="AA482">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB482">
         <v>8000</v>
@@ -45305,7 +45305,7 @@
         <v>178</v>
       </c>
       <c r="AA483">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB483">
         <v>8000</v>
@@ -45397,7 +45397,7 @@
         <v>178</v>
       </c>
       <c r="AA484">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB484">
         <v>8000</v>
@@ -45489,7 +45489,7 @@
         <v>178</v>
       </c>
       <c r="AA485">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB485">
         <v>8000</v>
@@ -45581,7 +45581,7 @@
         <v>178</v>
       </c>
       <c r="AA486">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB486">
         <v>8000</v>
@@ -45673,7 +45673,7 @@
         <v>178</v>
       </c>
       <c r="AA487">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB487">
         <v>8000</v>
@@ -45765,7 +45765,7 @@
         <v>178</v>
       </c>
       <c r="AA488">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB488">
         <v>8000</v>
@@ -45857,7 +45857,7 @@
         <v>178</v>
       </c>
       <c r="AA489">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB489">
         <v>8000</v>
@@ -45949,7 +45949,7 @@
         <v>178</v>
       </c>
       <c r="AA490">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB490">
         <v>8000</v>
@@ -46041,7 +46041,7 @@
         <v>178</v>
       </c>
       <c r="AA491">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB491">
         <v>8000</v>
@@ -46133,7 +46133,7 @@
         <v>178</v>
       </c>
       <c r="AA492">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB492">
         <v>8000</v>
@@ -46228,7 +46228,7 @@
         <v>178</v>
       </c>
       <c r="AA493">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB493">
         <v>8000</v>
@@ -46317,7 +46317,7 @@
         <v>178</v>
       </c>
       <c r="AA494">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB494">
         <v>8000</v>
@@ -46409,7 +46409,7 @@
         <v>178</v>
       </c>
       <c r="AA495">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB495">
         <v>8000</v>
@@ -46501,7 +46501,7 @@
         <v>178</v>
       </c>
       <c r="AA496">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB496">
         <v>8000</v>
@@ -46593,7 +46593,7 @@
         <v>178</v>
       </c>
       <c r="AA497">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB497">
         <v>8000</v>
@@ -46685,7 +46685,7 @@
         <v>178</v>
       </c>
       <c r="AA498">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB498">
         <v>8000</v>
@@ -46777,7 +46777,7 @@
         <v>178</v>
       </c>
       <c r="AA499">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB499">
         <v>8000</v>
@@ -46869,7 +46869,7 @@
         <v>178</v>
       </c>
       <c r="AA500">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB500">
         <v>8000</v>
@@ -46961,7 +46961,7 @@
         <v>178</v>
       </c>
       <c r="AA501">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB501">
         <v>8000</v>
@@ -47053,7 +47053,7 @@
         <v>178</v>
       </c>
       <c r="AA502">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB502">
         <v>8000</v>
@@ -47145,7 +47145,7 @@
         <v>178</v>
       </c>
       <c r="AA503">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB503">
         <v>8000</v>
@@ -47237,7 +47237,7 @@
         <v>178</v>
       </c>
       <c r="AA504">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB504">
         <v>8000</v>
@@ -47329,7 +47329,7 @@
         <v>178</v>
       </c>
       <c r="AA505">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB505">
         <v>8000</v>
@@ -47421,7 +47421,7 @@
         <v>178</v>
       </c>
       <c r="AA506">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB506">
         <v>8000</v>
@@ -47519,7 +47519,7 @@
         <v>178</v>
       </c>
       <c r="AA507">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB507">
         <v>8000</v>
@@ -47608,7 +47608,7 @@
         <v>178</v>
       </c>
       <c r="AA508">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB508">
         <v>8000</v>
@@ -47697,7 +47697,7 @@
         <v>178</v>
       </c>
       <c r="AA509">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB509">
         <v>8000</v>
@@ -47786,7 +47786,7 @@
         <v>178</v>
       </c>
       <c r="AA510">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB510">
         <v>8000</v>
@@ -47875,7 +47875,7 @@
         <v>178</v>
       </c>
       <c r="AA511">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB511">
         <v>8000</v>
@@ -47964,7 +47964,7 @@
         <v>178</v>
       </c>
       <c r="AA512">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB512">
         <v>8000</v>
@@ -48056,7 +48056,7 @@
         <v>178</v>
       </c>
       <c r="AA513">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB513">
         <v>8000</v>
@@ -48148,7 +48148,7 @@
         <v>178</v>
       </c>
       <c r="AA514">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB514">
         <v>8000</v>
@@ -48240,7 +48240,7 @@
         <v>178</v>
       </c>
       <c r="AA515">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB515">
         <v>8000</v>
@@ -48338,7 +48338,7 @@
         <v>178</v>
       </c>
       <c r="AA516">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB516">
         <v>8000</v>
@@ -48436,7 +48436,7 @@
         <v>178</v>
       </c>
       <c r="AA517">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB517">
         <v>8000</v>
@@ -48525,7 +48525,7 @@
         <v>178</v>
       </c>
       <c r="AA518">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB518">
         <v>8000</v>
@@ -48614,7 +48614,7 @@
         <v>178</v>
       </c>
       <c r="AA519">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB519">
         <v>8000</v>
@@ -48703,7 +48703,7 @@
         <v>178</v>
       </c>
       <c r="AA520">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB520">
         <v>8000</v>
@@ -48795,7 +48795,7 @@
         <v>178</v>
       </c>
       <c r="AA521">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB521">
         <v>8000</v>
@@ -48884,7 +48884,7 @@
         <v>178</v>
       </c>
       <c r="AA522">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB522">
         <v>8000</v>
@@ -48976,7 +48976,7 @@
         <v>178</v>
       </c>
       <c r="AA523">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB523">
         <v>8000</v>
@@ -49068,7 +49068,7 @@
         <v>178</v>
       </c>
       <c r="AA524">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB524">
         <v>8000</v>
@@ -49166,7 +49166,7 @@
         <v>178</v>
       </c>
       <c r="AA525">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB525">
         <v>8000</v>
@@ -49264,7 +49264,7 @@
         <v>178</v>
       </c>
       <c r="AA526">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB526">
         <v>8000</v>
@@ -49356,7 +49356,7 @@
         <v>178</v>
       </c>
       <c r="AA527">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB527">
         <v>8000</v>
@@ -49448,7 +49448,7 @@
         <v>178</v>
       </c>
       <c r="AA528">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB528">
         <v>8000</v>
@@ -49537,7 +49537,7 @@
         <v>178</v>
       </c>
       <c r="AA529">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB529">
         <v>8000</v>
@@ -49626,7 +49626,7 @@
         <v>178</v>
       </c>
       <c r="AA530">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB530">
         <v>8000</v>
@@ -49715,7 +49715,7 @@
         <v>178</v>
       </c>
       <c r="AA531">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB531">
         <v>8000</v>
@@ -49804,7 +49804,7 @@
         <v>178</v>
       </c>
       <c r="AA532">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB532">
         <v>8000</v>
@@ -49893,7 +49893,7 @@
         <v>178</v>
       </c>
       <c r="AA533">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB533">
         <v>8000</v>
@@ -49982,7 +49982,7 @@
         <v>178</v>
       </c>
       <c r="AA534">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB534">
         <v>8000</v>
@@ -50071,7 +50071,7 @@
         <v>178</v>
       </c>
       <c r="AA535">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB535">
         <v>8000</v>
@@ -50160,7 +50160,7 @@
         <v>178</v>
       </c>
       <c r="AA536">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB536">
         <v>8000</v>
@@ -50249,7 +50249,7 @@
         <v>178</v>
       </c>
       <c r="AA537">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB537">
         <v>8000</v>
@@ -50338,7 +50338,7 @@
         <v>178</v>
       </c>
       <c r="AA538">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB538">
         <v>8000</v>
@@ -50427,7 +50427,7 @@
         <v>178</v>
       </c>
       <c r="AA539">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB539">
         <v>8000</v>
@@ -50516,7 +50516,7 @@
         <v>178</v>
       </c>
       <c r="AA540">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB540">
         <v>8000</v>
@@ -50605,7 +50605,7 @@
         <v>178</v>
       </c>
       <c r="AA541">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB541">
         <v>8000</v>
@@ -50694,7 +50694,7 @@
         <v>178</v>
       </c>
       <c r="AA542">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB542">
         <v>8000</v>
@@ -50783,7 +50783,7 @@
         <v>178</v>
       </c>
       <c r="AA543">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB543">
         <v>8000</v>
@@ -50872,7 +50872,7 @@
         <v>178</v>
       </c>
       <c r="AA544">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB544">
         <v>8000</v>
@@ -50961,7 +50961,7 @@
         <v>178</v>
       </c>
       <c r="AA545">
-        <v>10</v>
+        <v>5.462962962962945</v>
       </c>
       <c r="AB545">
         <v>8000</v>
@@ -51053,7 +51053,7 @@
         <v>178</v>
       </c>
       <c r="AA546">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB546">
         <v>8000</v>
@@ -51145,7 +51145,7 @@
         <v>178</v>
       </c>
       <c r="AA547">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB547">
         <v>8000</v>
@@ -51237,7 +51237,7 @@
         <v>178</v>
       </c>
       <c r="AA548">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB548">
         <v>8000</v>
@@ -51332,7 +51332,7 @@
         <v>178</v>
       </c>
       <c r="AA549">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB549">
         <v>8000</v>
@@ -51424,7 +51424,7 @@
         <v>178</v>
       </c>
       <c r="AA550">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB550">
         <v>8000</v>
@@ -51513,7 +51513,7 @@
         <v>178</v>
       </c>
       <c r="AA551">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB551">
         <v>8000</v>
@@ -51602,7 +51602,7 @@
         <v>178</v>
       </c>
       <c r="AA552">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB552">
         <v>8000</v>
@@ -51691,7 +51691,7 @@
         <v>178</v>
       </c>
       <c r="AA553">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB553">
         <v>8000</v>
@@ -51783,7 +51783,7 @@
         <v>178</v>
       </c>
       <c r="AA554">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB554">
         <v>8000</v>
@@ -51875,7 +51875,7 @@
         <v>178</v>
       </c>
       <c r="AA555">
-        <v>10</v>
+        <v>19.60879629629628</v>
       </c>
       <c r="AB555">
         <v>8000</v>
@@ -51967,7 +51967,7 @@
         <v>178</v>
       </c>
       <c r="AA556">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB556">
         <v>8000</v>
@@ -52059,7 +52059,7 @@
         <v>178</v>
       </c>
       <c r="AA557">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB557">
         <v>8000</v>
@@ -52151,7 +52151,7 @@
         <v>178</v>
       </c>
       <c r="AA558">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB558">
         <v>8000</v>
@@ -52243,7 +52243,7 @@
         <v>178</v>
       </c>
       <c r="AA559">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB559">
         <v>8000</v>
@@ -52341,7 +52341,7 @@
         <v>178</v>
       </c>
       <c r="AA560">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB560">
         <v>8000</v>
@@ -52430,7 +52430,7 @@
         <v>178</v>
       </c>
       <c r="AA561">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB561">
         <v>8000</v>
@@ -52522,7 +52522,7 @@
         <v>178</v>
       </c>
       <c r="AA562">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB562">
         <v>8000</v>
@@ -52617,7 +52617,7 @@
         <v>178</v>
       </c>
       <c r="AA563">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB563">
         <v>8000</v>
@@ -52706,7 +52706,7 @@
         <v>178</v>
       </c>
       <c r="AA564">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB564">
         <v>8000</v>
@@ -52795,7 +52795,7 @@
         <v>178</v>
       </c>
       <c r="AA565">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB565">
         <v>8000</v>
@@ -52887,7 +52887,7 @@
         <v>178</v>
       </c>
       <c r="AA566">
-        <v>10</v>
+        <v>21.28240740740739</v>
       </c>
       <c r="AB566">
         <v>8000</v>
@@ -52979,7 +52979,7 @@
         <v>178</v>
       </c>
       <c r="AA567">
-        <v>10</v>
+        <v>21.28240740740739</v>
       </c>
       <c r="AB567">
         <v>8000</v>
@@ -53068,7 +53068,7 @@
         <v>178</v>
       </c>
       <c r="AA568">
-        <v>10</v>
+        <v>21.28240740740739</v>
       </c>
       <c r="AB568">
         <v>8000</v>
@@ -53160,7 +53160,7 @@
         <v>178</v>
       </c>
       <c r="AA569">
-        <v>10</v>
+        <v>21.28240740740739</v>
       </c>
       <c r="AB569">
         <v>8000</v>
@@ -53258,7 +53258,7 @@
         <v>178</v>
       </c>
       <c r="AA570">
-        <v>10</v>
+        <v>21.28240740740739</v>
       </c>
       <c r="AB570">
         <v>8000</v>
@@ -53347,7 +53347,7 @@
         <v>178</v>
       </c>
       <c r="AA571">
-        <v>10</v>
+        <v>21.28240740740739</v>
       </c>
       <c r="AB571">
         <v>8000</v>
@@ -53439,7 +53439,7 @@
         <v>178</v>
       </c>
       <c r="AA572">
-        <v>10</v>
+        <v>21.28240740740739</v>
       </c>
       <c r="AB572">
         <v>8000</v>
@@ -53534,7 +53534,7 @@
         <v>178</v>
       </c>
       <c r="AA573">
-        <v>10</v>
+        <v>21.28240740740739</v>
       </c>
       <c r="AB573">
         <v>8000</v>
@@ -53626,7 +53626,7 @@
         <v>178</v>
       </c>
       <c r="AA574">
-        <v>10</v>
+        <v>21.28240740740739</v>
       </c>
       <c r="AB574">
         <v>8000</v>
@@ -53715,7 +53715,7 @@
         <v>178</v>
       </c>
       <c r="AA575">
-        <v>10</v>
+        <v>21.28240740740739</v>
       </c>
       <c r="AB575">
         <v>8000</v>
@@ -53807,7 +53807,7 @@
         <v>178</v>
       </c>
       <c r="AA576">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB576">
         <v>8000</v>
@@ -53899,7 +53899,7 @@
         <v>178</v>
       </c>
       <c r="AA577">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB577">
         <v>8000</v>
@@ -53997,7 +53997,7 @@
         <v>178</v>
       </c>
       <c r="AA578">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB578">
         <v>8000</v>
@@ -54095,7 +54095,7 @@
         <v>178</v>
       </c>
       <c r="AA579">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB579">
         <v>8000</v>
@@ -54187,7 +54187,7 @@
         <v>178</v>
       </c>
       <c r="AA580">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB580">
         <v>8000</v>
@@ -54276,7 +54276,7 @@
         <v>178</v>
       </c>
       <c r="AA581">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB581">
         <v>8000</v>
@@ -54368,7 +54368,7 @@
         <v>178</v>
       </c>
       <c r="AA582">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB582">
         <v>8000</v>
@@ -54457,7 +54457,7 @@
         <v>178</v>
       </c>
       <c r="AA583">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB583">
         <v>8000</v>
@@ -54546,7 +54546,7 @@
         <v>178</v>
       </c>
       <c r="AA584">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB584">
         <v>8000</v>
@@ -54635,7 +54635,7 @@
         <v>178</v>
       </c>
       <c r="AA585">
-        <v>10</v>
+        <v>14.47727272727272</v>
       </c>
       <c r="AB585">
         <v>8000</v>

</xml_diff>